<commit_message>
chore(example): add nightfall portrait assets
</commit_message>
<xml_diff>
--- a/example/game_06_abyssal_nightfall/operators.xlsx
+++ b/example/game_06_abyssal_nightfall/operators.xlsx
@@ -531,7 +531,7 @@
         <v>passive:precision-lock</v>
       </c>
       <c r="N6" t="str">
-        <v>art/operators/sable.png</v>
+        <v>ui/assets/operators/sable.svg</v>
       </c>
     </row>
     <row r="7">
@@ -575,7 +575,7 @@
         <v>passive:seraph-ward</v>
       </c>
       <c r="N7" t="str">
-        <v>art/operators/iris.png</v>
+        <v>ui/assets/operators/iris.svg</v>
       </c>
     </row>
     <row r="8">
@@ -619,7 +619,7 @@
         <v>passive:undertow-grip</v>
       </c>
       <c r="N8" t="str">
-        <v>art/operators/marlow.png</v>
+        <v>ui/assets/operators/marlow.svg</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gaming (game_06): create more skills, and add assets of actor
</commit_message>
<xml_diff>
--- a/example/game_06_abyssal_nightfall/operators.xlsx
+++ b/example/game_06_abyssal_nightfall/operators.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:N8"/>
+  <dimension ref="A4:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -445,6 +445,12 @@
       <c r="N4" t="str">
         <v>string</v>
       </c>
+      <c r="O4" t="str">
+        <v>string</v>
+      </c>
+      <c r="P4" t="str">
+        <v>float</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -489,6 +495,12 @@
       <c r="N5" t="str">
         <v>portraitArt</v>
       </c>
+      <c r="O5" t="str">
+        <v>sprite</v>
+      </c>
+      <c r="P5" t="str">
+        <v>spriteScale</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -533,6 +545,12 @@
       <c r="N6" t="str">
         <v>ui/assets/operators/sable.svg</v>
       </c>
+      <c r="O6" t="str">
+        <v>ui/assets/actors/sable.png</v>
+      </c>
+      <c r="P6" t="str">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -577,6 +595,12 @@
       <c r="N7" t="str">
         <v>ui/assets/operators/iris.svg</v>
       </c>
+      <c r="O7" t="str">
+        <v>ui/assets/actors/iris.png</v>
+      </c>
+      <c r="P7" t="str">
+        <v>0.92</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -621,10 +645,16 @@
       <c r="N8" t="str">
         <v>ui/assets/operators/marlow.svg</v>
       </c>
+      <c r="O8" t="str">
+        <v>ui/assets/actors/marlow.png</v>
+      </c>
+      <c r="P8" t="str">
+        <v>0.95</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A4:N8"/>
+    <ignoredError numberStoredAsText="1" sqref="A4:P8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>